<commit_message>
Add illustrations to git
</commit_message>
<xml_diff>
--- a/data/illustrate_sd3.xlsx
+++ b/data/illustrate_sd3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE2B374-97E1-4799-847D-AAF0278EF518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A775B6D6-D75F-4048-B719-6FD30B2A9DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{9881D414-2483-48B2-8EA8-F4F1BE414074}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{9881D414-2483-48B2-8EA8-F4F1BE414074}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_deaths" sheetId="1" r:id="rId1"/>
@@ -27,21 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>ENGLAND + WALES</t>
-  </si>
-  <si>
-    <t>lower bound (2sd)</t>
-  </si>
-  <si>
-    <t>upper bound (2sd)</t>
-  </si>
-  <si>
-    <t>daily baseline</t>
-  </si>
-  <si>
-    <t>daily stdev</t>
   </si>
   <si>
     <t>Lower bound (2SD)</t>
@@ -62,10 +50,16 @@
     <t>Upper bound (daily 3SD)</t>
   </si>
   <si>
-    <t>weekly baseline</t>
+    <t>Weekly Baseline</t>
   </si>
   <si>
-    <t>weekly stdev</t>
+    <t>Daily Baseline</t>
+  </si>
+  <si>
+    <t>Daily SD</t>
+  </si>
+  <si>
+    <t>Weekly SD</t>
   </si>
 </sst>
 </file>
@@ -3834,8 +3828,208 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>weekly_deaths!$A$54</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Weekly Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>weekly_deaths!$B$54:$BA$54</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>12123.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12004.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11616.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11257.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11240.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11052.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10872.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10727.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10732.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10459</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10262.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10130.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10119.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10028.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9904.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9676.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9507.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9479.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9323.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9296.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9061.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8982</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8992.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8993.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8905.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8953.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8707.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8879.7000000000007</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8887.6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8658.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8750.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8740.4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8745.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8767</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8766.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8852.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9036.1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9174.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9304</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9405.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9558.7000000000007</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9594.4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9774.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9783.1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9853.4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>9933.1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10135.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10508.5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>10873.3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>11308.4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>11567</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3890-468E-B723-6D4C29EB6FE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="16"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>weekly_deaths!$A$52</c:f>
@@ -4018,7 +4212,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="13"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>weekly_deaths!$A$57</c:f>
@@ -4217,7 +4411,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="12"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>weekly_deaths!$A$56</c:f>
@@ -4416,7 +4610,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="11"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>weekly_deaths!$A$59</c:f>
@@ -4617,7 +4811,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>weekly_deaths!$A$58</c:f>
@@ -4818,7 +5012,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="15"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>weekly_deaths!$A$66</c:f>
@@ -5017,7 +5211,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="14"/>
-          <c:order val="6"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>weekly_deaths!$A$65</c:f>
@@ -7781,7 +7975,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="AB38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A68" sqref="A68"/>
+      <selection pane="bottomRight" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16330,10 +16524,10 @@
     </row>
     <row r="54" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B54" s="2">
-        <f t="shared" ref="B54:AG54" si="1">AVERAGE(B$42:B$51)</f>
+        <f t="shared" ref="B54:Z54" si="1">AVERAGE(B$42:B$51)</f>
         <v>12123.6</v>
       </c>
       <c r="C54" s="2">
@@ -16544,10 +16738,10 @@
     </row>
     <row r="55" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B55" s="2">
-        <f t="shared" ref="B55:AG55" si="3">STDEV(B$42:B$51)</f>
+        <f t="shared" ref="B55:Z55" si="3">STDEV(B$42:B$51)</f>
         <v>1310.6822820365182</v>
       </c>
       <c r="C55" s="2">
@@ -16758,7 +16952,7 @@
     </row>
     <row r="56" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B56" s="2">
         <f t="shared" ref="B56:Z56" si="5">B54-2*B55</f>
@@ -16972,7 +17166,7 @@
     </row>
     <row r="57" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B57" s="2">
         <f t="shared" ref="B57:Z57" si="7">B54+2*B55</f>
@@ -17186,7 +17380,7 @@
     </row>
     <row r="58" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B58" s="2">
         <f t="shared" ref="B58:Z58" si="9">B54-3*B55</f>
@@ -17400,7 +17594,7 @@
     </row>
     <row r="59" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B59" s="2">
         <f t="shared" ref="B59:Z59" si="11">B54+3*B55</f>
@@ -17669,7 +17863,7 @@
     </row>
     <row r="61" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B61" s="3">
         <v>12151.3</v>
@@ -17831,7 +18025,7 @@
     </row>
     <row r="62" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B62" s="3">
         <v>1380.0668000000001</v>
@@ -18421,7 +18615,7 @@
     </row>
     <row r="65" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B65" s="2">
         <f t="shared" ref="B65:Z65" si="66">B61-3*B62</f>
@@ -18635,7 +18829,7 @@
     </row>
     <row r="66" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B66" s="2">
         <f t="shared" ref="B66:Z66" si="68">B61+3*B62</f>
@@ -18857,7 +19051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CF2BBA-FD0C-4963-AD0E-24A5A8CA29DE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
@@ -18872,8 +19066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BE2D47-24FD-4B80-AC0C-7E3DEE79A7E6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add note about 4 occurences of breaching 2SD
</commit_message>
<xml_diff>
--- a/data/illustrate_sd3.xlsx
+++ b/data/illustrate_sd3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EF72B8-C8B8-45FF-82D3-D9AC0D801B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DEFB0F-F7CB-48A0-B6C8-90F43582F58E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{9881D414-2483-48B2-8EA8-F4F1BE414074}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{9881D414-2483-48B2-8EA8-F4F1BE414074}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_deaths" sheetId="1" r:id="rId1"/>
@@ -6877,56 +6877,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Connector 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DE38EC7-7596-4BBA-89CB-257306EE13C8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4848225" y="1419225"/>
-          <a:ext cx="57150" cy="5219700"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6934,12 +6884,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.3584</cdr:x>
-      <cdr:y>0.29829</cdr:y>
+      <cdr:x>0.49445</cdr:x>
+      <cdr:y>0.46912</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.60428</cdr:x>
-      <cdr:y>0.37188</cdr:y>
+      <cdr:x>0.74033</cdr:x>
+      <cdr:y>0.56242</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -6954,8 +6904,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4943177" y="2162176"/>
-          <a:ext cx="3391197" cy="533400"/>
+          <a:off x="6819549" y="3400412"/>
+          <a:ext cx="3391227" cy="676288"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -6979,7 +6929,17 @@
                 <a:schemeClr val="tx2"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> look more like weekly 4SD after week 17</a:t>
+            <a:t> look more like weekly 4SD after week 17.</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>This is due to daily data being somewhat "noisy".</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1200">
             <a:solidFill>
@@ -6992,12 +6952,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.65838</cdr:x>
-      <cdr:y>0.47481</cdr:y>
+      <cdr:x>0.70672</cdr:x>
+      <cdr:y>0.38545</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.91851</cdr:x>
-      <cdr:y>0.54928</cdr:y>
+      <cdr:x>0.96685</cdr:x>
+      <cdr:y>0.45992</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -7012,8 +6972,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="9080500" y="3441701"/>
-          <a:ext cx="3587749" cy="539750"/>
+          <a:off x="9747259" y="2793972"/>
+          <a:ext cx="3587765" cy="539797"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -7093,7 +7053,7 @@
                 <a:schemeClr val="tx2"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>During these 10 years,</a:t>
+            <a:t>During 2010-2019,</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -7103,7 +7063,23 @@
                 <a:schemeClr val="tx2"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>none have </a:t>
+            <a:t>no</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> weeks</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1200" baseline="0">
@@ -7124,12 +7100,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.40769</cdr:x>
-      <cdr:y>0.47744</cdr:y>
+      <cdr:x>0.38283</cdr:x>
+      <cdr:y>0.38677</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.6174</cdr:x>
-      <cdr:y>0.6071</cdr:y>
+      <cdr:x>0.65884</cdr:x>
+      <cdr:y>0.51643</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -7144,8 +7120,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5622925" y="3460750"/>
-          <a:ext cx="2892424" cy="939800"/>
+          <a:off x="5280041" y="2803510"/>
+          <a:ext cx="3806808" cy="939844"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -7225,7 +7201,7 @@
                 <a:schemeClr val="tx2"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>In previous years it was rare to exceed 2SD and it was only ever for one week at a time.</a:t>
+            <a:t>During 2010-2019 it was rare to exceed 2SD (only 4 times) and it was only ever once in a single year.</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -7281,57 +7257,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.35499</cdr:x>
-      <cdr:y>0.13009</cdr:y>
+      <cdr:x>0.541</cdr:x>
+      <cdr:y>0.4078</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.35827</cdr:x>
-      <cdr:y>0.91897</cdr:y>
-    </cdr:to>
-    <cdr:cxnSp macro="">
-      <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="2" name="Straight Connector 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DE38EC7-7596-4BBA-89CB-257306EE13C8}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvCxnSpPr/>
-      </cdr:nvCxnSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="4895882" y="942975"/>
-          <a:ext cx="45253" cy="5718175"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:style>
-        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </cdr:style>
-    </cdr:cxnSp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.73023</cdr:x>
-      <cdr:y>0.40517</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.93996</cdr:x>
-      <cdr:y>0.53482</cdr:y>
+      <cdr:x>0.75073</cdr:x>
+      <cdr:y>0.53745</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -7346,8 +7277,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="10071101" y="2936875"/>
-          <a:ext cx="2892424" cy="939800"/>
+          <a:off x="7461190" y="2955934"/>
+          <a:ext cx="2892512" cy="939772"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -7448,19 +7379,19 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.39942</cdr:x>
-      <cdr:y>0.3237</cdr:y>
+      <cdr:x>0.43257</cdr:x>
+      <cdr:y>0.31976</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.64531</cdr:x>
-      <cdr:y>0.39728</cdr:y>
+      <cdr:x>0.70998</cdr:x>
+      <cdr:y>0.44941</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="8" name="TextBox 1">
+        <cdr:cNvPr id="9" name="TextBox 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EE1D903-BB2B-4632-81B5-F666EB51BC33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EEC03B6-9B5A-4D61-912B-0CEDD8DD9F55}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -7468,8 +7399,249 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5508625" y="2346325"/>
-          <a:ext cx="3391197" cy="533400"/>
+          <a:off x="5965882" y="2317759"/>
+          <a:ext cx="3825818" cy="939772"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>During 2010-2019 it was rare to exceed 2SD (only 4 times) and it was only ever once in a single year.</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76956</cdr:x>
+      <cdr:y>0.32238</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91302</cdr:x>
+      <cdr:y>0.39685</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D918341-E1E6-4263-8A2A-949E44223FCA}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="10613411" y="2336800"/>
+          <a:ext cx="1978640" cy="539797"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>During 2010-2019,</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>no weeks </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>exceeded 3SD.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1200">
+            <a:solidFill>
+              <a:schemeClr val="tx2"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53064</cdr:x>
+      <cdr:y>0.74157</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.77653</cdr:x>
+      <cdr:y>0.83487</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EBCD759-D6CC-47EE-AD5E-7863D0F45924}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7318375" y="5375275"/>
+          <a:ext cx="3391227" cy="676288"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -7557,122 +7729,23 @@
                 <a:schemeClr val="tx2"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> look more like weekly 4SD after week 17</a:t>
+            <a:t> look more like weekly 4SD after week 17.</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>This is due to daily data being somewhat "noisy".</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1200">
             <a:solidFill>
               <a:schemeClr val="tx2"/>
             </a:solidFill>
           </a:endParaRPr>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.47194</cdr:x>
-      <cdr:y>0.40517</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.68166</cdr:x>
-      <cdr:y>0.53482</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="9" name="TextBox 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EEC03B6-9B5A-4D61-912B-0CEDD8DD9F55}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="6508750" y="2936875"/>
-          <a:ext cx="2892424" cy="939800"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>In previous years it was rare to exceed 2SD and it was only ever for one week at a time.</a:t>
-          </a:r>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -12563,13 +12636,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D83C0BF-E992-4D0C-860A-5F1936D992C3}">
-  <dimension ref="A1:BB16"/>
+  <dimension ref="A1:BB15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14936,494 +15009,280 @@
       <c r="BB11" s="2"/>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>2020</v>
-      </c>
-      <c r="B12" s="2">
-        <f>IF(weekly_deaths!B12&gt;weekly_deaths!B$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <f>IF(weekly_deaths!C12&gt;weekly_deaths!C$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <f>IF(weekly_deaths!D12&gt;weekly_deaths!D$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <f>IF(weekly_deaths!E12&gt;weekly_deaths!E$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <f>IF(weekly_deaths!F12&gt;weekly_deaths!F$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <f>IF(weekly_deaths!G12&gt;weekly_deaths!G$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <f>IF(weekly_deaths!H12&gt;weekly_deaths!H$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <f>IF(weekly_deaths!I12&gt;weekly_deaths!I$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <f>IF(weekly_deaths!J12&gt;weekly_deaths!J$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="2">
-        <f>IF(weekly_deaths!K12&gt;weekly_deaths!K$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="2">
-        <f>IF(weekly_deaths!L12&gt;weekly_deaths!L$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="2">
-        <f>IF(weekly_deaths!M12&gt;weekly_deaths!M$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="2">
-        <f>IF(weekly_deaths!N12&gt;weekly_deaths!N$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O12" s="2">
-        <f>IF(weekly_deaths!O12&gt;weekly_deaths!O$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="P12" s="2">
-        <f>IF(weekly_deaths!P12&gt;weekly_deaths!P$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Q12" s="2">
-        <f>IF(weekly_deaths!Q12&gt;weekly_deaths!Q$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="R12" s="2">
-        <f>IF(weekly_deaths!R12&gt;weekly_deaths!R$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="S12" s="2">
-        <f>IF(weekly_deaths!S12&gt;weekly_deaths!S$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="T12" s="2">
-        <f>IF(weekly_deaths!T12&gt;weekly_deaths!T$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U12" s="2">
-        <f>IF(weekly_deaths!U12&gt;weekly_deaths!U$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="V12" s="2">
-        <f>IF(weekly_deaths!V12&gt;weekly_deaths!V$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="W12" s="2">
-        <f>IF(weekly_deaths!W12&gt;weekly_deaths!W$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="X12" s="2">
-        <f>IF(weekly_deaths!X12&gt;weekly_deaths!X$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Y12" s="2">
-        <f>IF(weekly_deaths!Y12&gt;weekly_deaths!Y$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z12" s="2">
-        <f>IF(weekly_deaths!Z12&gt;weekly_deaths!Z$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA12" s="2">
-        <f>IF(weekly_deaths!AA12&gt;weekly_deaths!AA$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AB12" s="2">
-        <f>IF(weekly_deaths!AB12&gt;weekly_deaths!AB$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC12" s="2">
-        <f>IF(weekly_deaths!AC12&gt;weekly_deaths!AC$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AD12" s="2">
-        <f>IF(weekly_deaths!AD12&gt;weekly_deaths!AD$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE12" s="2">
-        <f>IF(weekly_deaths!AE12&gt;weekly_deaths!AE$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AF12" s="2">
-        <f>IF(weekly_deaths!AF12&gt;weekly_deaths!AF$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AG12" s="2">
-        <f>IF(weekly_deaths!AG12&gt;weekly_deaths!AG$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AH12" s="2">
-        <f>IF(weekly_deaths!AH12&gt;weekly_deaths!AH$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AI12" s="2">
-        <f>IF(weekly_deaths!AI12&gt;weekly_deaths!AI$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="2">
-        <f>IF(weekly_deaths!AJ12&gt;weekly_deaths!AJ$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AK12" s="2">
-        <f>IF(weekly_deaths!AK12&gt;weekly_deaths!AK$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AL12" s="2">
-        <f>IF(weekly_deaths!AL12&gt;weekly_deaths!AL$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AM12" s="2">
-        <f>IF(weekly_deaths!AM12&gt;weekly_deaths!AM$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AN12" s="2">
-        <f>IF(weekly_deaths!AN12&gt;weekly_deaths!AN$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AO12" s="2">
-        <f>IF(weekly_deaths!AO12&gt;weekly_deaths!AO$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AP12" s="2">
-        <f>IF(weekly_deaths!AP12&gt;weekly_deaths!AP$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="2">
-        <f>IF(weekly_deaths!AQ12&gt;weekly_deaths!AQ$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AR12" s="2">
-        <f>IF(weekly_deaths!AR12&gt;weekly_deaths!AR$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AS12" s="2">
-        <f>IF(weekly_deaths!AS12&gt;weekly_deaths!AS$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AT12" s="2">
-        <f>IF(weekly_deaths!AT12&gt;weekly_deaths!AT$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AU12" s="2">
-        <f>IF(weekly_deaths!AU12&gt;weekly_deaths!AU$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AV12" s="2">
-        <f>IF(weekly_deaths!AV12&gt;weekly_deaths!AV$17,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AW12" s="2">
-        <f>IF(weekly_deaths!AW12&gt;weekly_deaths!AW$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AX12" s="2">
-        <f>IF(weekly_deaths!AX12&gt;weekly_deaths!AX$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AY12" s="2">
-        <f>IF(weekly_deaths!AY12&gt;weekly_deaths!AY$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AZ12" s="2">
-        <f>IF(weekly_deaths!AZ12&gt;weekly_deaths!AZ$17,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BA12" s="2">
-        <f>IF(weekly_deaths!BA12&gt;weekly_deaths!BA$17,1,0)</f>
-        <v>0</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="2"/>
+      <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2"/>
+      <c r="AZ12" s="2"/>
+      <c r="BA12" s="2"/>
       <c r="BB12" s="2"/>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
-      <c r="AF13" s="2"/>
-      <c r="AG13" s="2"/>
-      <c r="AH13" s="2"/>
-      <c r="AI13" s="2"/>
-      <c r="AJ13" s="2"/>
-      <c r="AK13" s="2"/>
-      <c r="AL13" s="2"/>
-      <c r="AM13" s="2"/>
-      <c r="AN13" s="2"/>
-      <c r="AO13" s="2"/>
-      <c r="AP13" s="2"/>
-      <c r="AQ13" s="2"/>
-      <c r="AR13" s="2"/>
-      <c r="AS13" s="2"/>
-      <c r="AT13" s="2"/>
-      <c r="AU13" s="2"/>
-      <c r="AV13" s="2"/>
-      <c r="AW13" s="2"/>
-      <c r="AX13" s="2"/>
-      <c r="AY13" s="2"/>
-      <c r="AZ13" s="2"/>
-      <c r="BA13" s="2"/>
-      <c r="BB13" s="2"/>
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <f>SUM(B2:B11)</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <f>SUM(C2:C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <f>SUM(D2:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <f>SUM(E2:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <f>SUM(F2:F11)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <f>SUM(G2:G11)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <f>SUM(H2:H11)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f>SUM(I2:I11)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <f>SUM(J2:J11)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <f>SUM(K2:K11)</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <f>SUM(L2:L11)</f>
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <f>SUM(M2:M11)</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <f>SUM(N2:N11)</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <f>SUM(O2:O11)</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <f>SUM(P2:P11)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <f>SUM(Q2:Q11)</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <f>SUM(R2:R11)</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <f>SUM(S2:S11)</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <f>SUM(T2:T11)</f>
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <f>SUM(U2:U11)</f>
+        <v>0</v>
+      </c>
+      <c r="V13" s="2">
+        <f>SUM(V2:V11)</f>
+        <v>0</v>
+      </c>
+      <c r="W13" s="2">
+        <f>SUM(W2:W11)</f>
+        <v>0</v>
+      </c>
+      <c r="X13" s="2">
+        <f>SUM(X2:X11)</f>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="2">
+        <f>SUM(Y2:Y11)</f>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="2">
+        <f>SUM(Z2:Z11)</f>
+        <v>1</v>
+      </c>
+      <c r="AA13" s="2">
+        <f>SUM(AA2:AA11)</f>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <f>SUM(AB2:AB11)</f>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="2">
+        <f>SUM(AC2:AC11)</f>
+        <v>0</v>
+      </c>
+      <c r="AD13" s="2">
+        <f>SUM(AD2:AD11)</f>
+        <v>1</v>
+      </c>
+      <c r="AE13" s="2">
+        <f>SUM(AE2:AE11)</f>
+        <v>0</v>
+      </c>
+      <c r="AF13" s="2">
+        <f>SUM(AF2:AF11)</f>
+        <v>0</v>
+      </c>
+      <c r="AG13" s="2">
+        <f>SUM(AG2:AG11)</f>
+        <v>0</v>
+      </c>
+      <c r="AH13" s="2">
+        <f>SUM(AH2:AH11)</f>
+        <v>0</v>
+      </c>
+      <c r="AI13" s="2">
+        <f>SUM(AI2:AI11)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="2">
+        <f>SUM(AJ2:AJ11)</f>
+        <v>0</v>
+      </c>
+      <c r="AK13" s="2">
+        <f>SUM(AK2:AK11)</f>
+        <v>0</v>
+      </c>
+      <c r="AL13" s="2">
+        <f>SUM(AL2:AL11)</f>
+        <v>0</v>
+      </c>
+      <c r="AM13" s="2">
+        <f>SUM(AM2:AM11)</f>
+        <v>0</v>
+      </c>
+      <c r="AN13" s="2">
+        <f>SUM(AN2:AN11)</f>
+        <v>0</v>
+      </c>
+      <c r="AO13" s="2">
+        <f>SUM(AO2:AO11)</f>
+        <v>0</v>
+      </c>
+      <c r="AP13" s="2">
+        <f>SUM(AP2:AP11)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="2">
+        <f>SUM(AQ2:AQ11)</f>
+        <v>0</v>
+      </c>
+      <c r="AR13" s="2">
+        <f>SUM(AR2:AR11)</f>
+        <v>0</v>
+      </c>
+      <c r="AS13" s="2">
+        <f>SUM(AS2:AS11)</f>
+        <v>0</v>
+      </c>
+      <c r="AT13" s="2">
+        <f>SUM(AT2:AT11)</f>
+        <v>0</v>
+      </c>
+      <c r="AU13" s="2">
+        <f>SUM(AU2:AU11)</f>
+        <v>0</v>
+      </c>
+      <c r="AV13" s="2">
+        <f>SUM(AV2:AV11)</f>
+        <v>0</v>
+      </c>
+      <c r="AW13" s="2">
+        <f>SUM(AW2:AW11)</f>
+        <v>0</v>
+      </c>
+      <c r="AX13" s="2">
+        <f>SUM(AX2:AX11)</f>
+        <v>0</v>
+      </c>
+      <c r="AY13" s="2">
+        <f>SUM(AY2:AY11)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ13" s="2">
+        <f>SUM(AZ2:AZ11)</f>
+        <v>0</v>
+      </c>
+      <c r="BA13" s="2">
+        <f>SUM(BA2:BA11)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2">
-        <f>SUM(B2:B12)</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <f>SUM(C2:C12)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <f>SUM(D2:D12)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <f>SUM(E2:E12)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <f>SUM(F2:F12)</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <f>SUM(G2:G12)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <f>SUM(H2:H12)</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <f>SUM(I2:I12)</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <f>SUM(J2:J12)</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <f>SUM(K2:K12)</f>
-        <v>1</v>
-      </c>
-      <c r="L14" s="2">
-        <f>SUM(L2:L12)</f>
-        <v>1</v>
-      </c>
-      <c r="M14" s="2">
-        <f>SUM(M2:M12)</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
-        <f>SUM(N2:N12)</f>
-        <v>1</v>
-      </c>
-      <c r="O14" s="2">
-        <f>SUM(O2:O12)</f>
-        <v>1</v>
-      </c>
-      <c r="P14" s="2">
-        <f>SUM(P2:P12)</f>
-        <v>1</v>
-      </c>
-      <c r="Q14" s="2">
-        <f>SUM(Q2:Q12)</f>
-        <v>1</v>
-      </c>
-      <c r="R14" s="2">
-        <f>SUM(R2:R12)</f>
-        <v>1</v>
-      </c>
-      <c r="S14" s="2">
-        <f>SUM(S2:S12)</f>
-        <v>1</v>
-      </c>
-      <c r="T14" s="2">
-        <f>SUM(T2:T12)</f>
-        <v>1</v>
-      </c>
-      <c r="U14" s="2">
-        <f>SUM(U2:U12)</f>
-        <v>1</v>
-      </c>
-      <c r="V14" s="2">
-        <f>SUM(V2:V12)</f>
-        <v>1</v>
-      </c>
-      <c r="W14" s="2">
-        <f>SUM(W2:W12)</f>
-        <v>1</v>
-      </c>
-      <c r="X14" s="2">
-        <f>SUM(X2:X12)</f>
-        <v>1</v>
-      </c>
-      <c r="Y14" s="2">
-        <f>SUM(Y2:Y12)</f>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="2">
-        <f>SUM(Z2:Z12)</f>
-        <v>1</v>
-      </c>
-      <c r="AA14" s="2">
-        <f>SUM(AA2:AA12)</f>
-        <v>1</v>
-      </c>
-      <c r="AB14" s="2">
-        <f>SUM(AB2:AB12)</f>
-        <v>0</v>
-      </c>
-      <c r="AC14" s="2">
-        <f>SUM(AC2:AC12)</f>
-        <v>0</v>
-      </c>
-      <c r="AD14" s="2">
-        <f>SUM(AD2:AD12)</f>
-        <v>1</v>
-      </c>
-      <c r="AE14" s="2">
-        <f>SUM(AE2:AE12)</f>
-        <v>0</v>
-      </c>
-      <c r="AF14" s="2">
-        <f>SUM(AF2:AF12)</f>
-        <v>0</v>
-      </c>
-      <c r="AG14" s="2">
-        <f>SUM(AG2:AG12)</f>
-        <v>0</v>
-      </c>
-      <c r="AH14" s="2">
-        <f>SUM(AH2:AH12)</f>
-        <v>1</v>
-      </c>
-      <c r="AI14" s="2">
-        <f>SUM(AI2:AI12)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="2">
-        <f>SUM(AJ2:AJ12)</f>
-        <v>0</v>
-      </c>
-      <c r="AK14" s="2">
-        <f>SUM(AK2:AK12)</f>
-        <v>0</v>
-      </c>
-      <c r="AL14" s="2">
-        <f>SUM(AL2:AL12)</f>
-        <v>0</v>
-      </c>
-      <c r="AM14" s="2">
-        <f>SUM(AM2:AM12)</f>
-        <v>0</v>
-      </c>
-      <c r="AN14" s="2">
-        <f>SUM(AN2:AN12)</f>
-        <v>0</v>
-      </c>
-      <c r="AO14" s="2">
-        <f>SUM(AO2:AO12)</f>
-        <v>1</v>
-      </c>
-      <c r="AP14" s="2">
-        <f>SUM(AP2:AP12)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="2">
-        <f>SUM(AQ2:AQ12)</f>
-        <v>0</v>
-      </c>
-      <c r="AR14" s="2">
-        <f>SUM(AR2:AR12)</f>
-        <v>1</v>
-      </c>
-      <c r="AS14" s="2">
-        <f>SUM(AS2:AS12)</f>
-        <v>1</v>
-      </c>
-      <c r="AT14" s="2">
-        <f>SUM(AT2:AT12)</f>
-        <v>1</v>
-      </c>
-      <c r="AU14" s="2">
-        <f>SUM(AU2:AU12)</f>
-        <v>1</v>
-      </c>
-      <c r="AV14" s="2">
-        <f>SUM(AV2:AV12)</f>
-        <v>1</v>
-      </c>
-      <c r="AW14" s="2">
-        <f>SUM(AW2:AW12)</f>
-        <v>0</v>
-      </c>
-      <c r="AX14" s="2">
-        <f>SUM(AX2:AX12)</f>
-        <v>0</v>
-      </c>
-      <c r="AY14" s="2">
-        <f>SUM(AY2:AY12)</f>
-        <v>0</v>
-      </c>
-      <c r="AZ14" s="2">
-        <f>SUM(AZ2:AZ12)</f>
-        <v>0</v>
-      </c>
-      <c r="BA14" s="2">
-        <f>SUM(BA2:BA12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="2">
-        <f>SUM(B14:BA14)</f>
-        <v>23</v>
+      <c r="B15" s="2">
+        <f>SUM(B13:BA13)</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -17924,211 +17783,211 @@
         <v>11</v>
       </c>
       <c r="B14" s="2">
-        <f>SUM(B2:B12)</f>
+        <f t="shared" ref="B14:AG14" si="1">SUM(B2:B12)</f>
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <f>SUM(C2:C12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D14" s="2">
-        <f>SUM(D2:D12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <f>SUM(E2:E12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <f>SUM(F2:F12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <f>SUM(G2:G12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H14" s="2">
-        <f>SUM(H2:H12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I14" s="2">
-        <f>SUM(I2:I12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J14" s="2">
-        <f>SUM(J2:J12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K14" s="2">
-        <f>SUM(K2:K12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L14" s="2">
-        <f>SUM(L2:L12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M14" s="2">
-        <f>SUM(M2:M12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N14" s="2">
-        <f>SUM(N2:N12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <f>SUM(O2:O12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P14" s="2">
-        <f>SUM(P2:P12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q14" s="2">
-        <f>SUM(Q2:Q12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <f>SUM(R2:R12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S14" s="2">
-        <f>SUM(S2:S12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T14" s="2">
-        <f>SUM(T2:T12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U14" s="2">
-        <f>SUM(U2:U12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V14" s="2">
-        <f>SUM(V2:V12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W14" s="2">
-        <f>SUM(W2:W12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X14" s="2">
-        <f>SUM(X2:X12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y14" s="2">
-        <f>SUM(Y2:Y12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z14" s="2">
-        <f>SUM(Z2:Z12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA14" s="2">
-        <f>SUM(AA2:AA12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB14" s="2">
-        <f>SUM(AB2:AB12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC14" s="2">
-        <f>SUM(AC2:AC12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD14" s="2">
-        <f>SUM(AD2:AD12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE14" s="2">
-        <f>SUM(AE2:AE12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF14" s="2">
-        <f>SUM(AF2:AF12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG14" s="2">
-        <f>SUM(AG2:AG12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH14" s="2">
-        <f>SUM(AH2:AH12)</f>
+        <f t="shared" ref="AH14:BA14" si="2">SUM(AH2:AH12)</f>
         <v>0</v>
       </c>
       <c r="AI14" s="2">
-        <f>SUM(AI2:AI12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="2">
-        <f>SUM(AJ2:AJ12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK14" s="2">
-        <f>SUM(AK2:AK12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AL14" s="2">
-        <f>SUM(AL2:AL12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM14" s="2">
-        <f>SUM(AM2:AM12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AN14" s="2">
-        <f>SUM(AN2:AN12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AO14" s="2">
-        <f>SUM(AO2:AO12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AP14" s="2">
-        <f>SUM(AP2:AP12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AQ14" s="2">
-        <f>SUM(AQ2:AQ12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AR14" s="2">
-        <f>SUM(AR2:AR12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AS14" s="2">
-        <f>SUM(AS2:AS12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AT14" s="2">
-        <f>SUM(AT2:AT12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AU14" s="2">
-        <f>SUM(AU2:AU12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AV14" s="2">
-        <f>SUM(AV2:AV12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AW14" s="2">
-        <f>SUM(AW2:AW12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AX14" s="2">
-        <f>SUM(AX2:AX12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AY14" s="2">
-        <f>SUM(AY2:AY12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AZ14" s="2">
-        <f>SUM(AZ2:AZ12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BA14" s="2">
-        <f>SUM(BA2:BA12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -18155,8 +18014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CF2BBA-FD0C-4963-AD0E-24A5A8CA29DE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18170,8 +18029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BE2D47-24FD-4B80-AC0C-7E3DEE79A7E6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X21" sqref="X21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>